<commit_message>
pageup、pagedown按钮 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_ホワイトボート_トラブル一覧_new.xlsx
+++ b/test_物件管理/test_ホワイトボート_トラブル一覧_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="792" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="792" firstSheet="1" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="IN_FORM_006" sheetId="23" r:id="rId12"/>
     <sheet name="EXPECT_006" sheetId="24" r:id="rId13"/>
     <sheet name="テストケース" sheetId="3" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="26" r:id="rId15"/>
   </sheets>
   <calcPr calcId="125725" calcMode="manual" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3425" uniqueCount="645">
   <si>
     <t>URL:</t>
   </si>
@@ -2341,6 +2342,30 @@
   <si>
     <t>变更</t>
     <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGEUP</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGEUP</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL:</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>/contract/subscription/2/change/</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGEDOWN</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet1</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -3576,7 +3601,7 @@
   <dimension ref="A1:KP147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -17332,8 +17357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="I24:J24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -17378,11 +17403,8 @@
       <c r="B5" s="182" t="s">
         <v>576</v>
       </c>
-      <c r="C5" s="68" t="s">
-        <v>367</v>
-      </c>
-      <c r="D5" s="68" t="s">
-        <v>230</v>
+      <c r="D5" s="182" t="s">
+        <v>644</v>
       </c>
       <c r="I5" s="63"/>
       <c r="J5" s="63"/>
@@ -17414,15 +17436,6 @@
       <c r="B7" s="182" t="s">
         <v>577</v>
       </c>
-      <c r="D7" s="68" t="s">
-        <v>435</v>
-      </c>
-      <c r="E7" s="68" t="s">
-        <v>349</v>
-      </c>
-      <c r="F7" s="68" t="s">
-        <v>350</v>
-      </c>
       <c r="I7" s="63"/>
       <c r="J7" s="63"/>
       <c r="K7" s="63"/>
@@ -17438,15 +17451,6 @@
       <c r="B8" s="182" t="s">
         <v>578</v>
       </c>
-      <c r="D8" s="68" t="s">
-        <v>438</v>
-      </c>
-      <c r="E8" s="68" t="s">
-        <v>359</v>
-      </c>
-      <c r="F8" s="68" t="s">
-        <v>360</v>
-      </c>
       <c r="I8" s="63"/>
       <c r="J8" s="63"/>
       <c r="K8" s="63"/>
@@ -17477,15 +17481,6 @@
       <c r="B10" s="182" t="s">
         <v>580</v>
       </c>
-      <c r="D10" s="68" t="s">
-        <v>467</v>
-      </c>
-      <c r="E10" s="68" t="s">
-        <v>468</v>
-      </c>
-      <c r="F10" s="68" t="s">
-        <v>469</v>
-      </c>
       <c r="I10" s="63"/>
       <c r="J10" s="63"/>
       <c r="K10" s="63"/>
@@ -17546,23 +17541,16 @@
       <c r="B14" s="182" t="s">
         <v>627</v>
       </c>
-      <c r="D14" s="182" t="s">
-        <v>636</v>
-      </c>
-      <c r="E14" s="68" t="s">
-        <v>525</v>
-      </c>
-      <c r="F14" s="68" t="s">
-        <v>526</v>
-      </c>
       <c r="I14" s="63"/>
       <c r="J14" s="63"/>
       <c r="K14" s="63"/>
       <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
+      <c r="M14" s="68" t="s">
+        <v>367</v>
+      </c>
+      <c r="N14" s="68" t="s">
+        <v>230</v>
+      </c>
       <c r="Q14" s="63"/>
     </row>
     <row r="15" spans="1:17" s="68" customFormat="1">
@@ -17571,10 +17559,6 @@
         <v>528</v>
       </c>
       <c r="I15" s="63"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="63"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
       <c r="Q15" s="63"/>
     </row>
     <row r="16" spans="1:17" s="68" customFormat="1">
@@ -17583,10 +17567,15 @@
         <v>584</v>
       </c>
       <c r="I16" s="63"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
+      <c r="N16" s="68" t="s">
+        <v>435</v>
+      </c>
+      <c r="O16" s="68" t="s">
+        <v>349</v>
+      </c>
+      <c r="P16" s="68" t="s">
+        <v>350</v>
+      </c>
       <c r="Q16" s="63"/>
     </row>
     <row r="17" spans="1:17" s="68" customFormat="1">
@@ -17594,21 +17583,16 @@
       <c r="B17" s="182" t="s">
         <v>585</v>
       </c>
-      <c r="C17" s="182"/>
-      <c r="D17" s="182" t="s">
-        <v>586</v>
-      </c>
-      <c r="E17" s="182" t="s">
-        <v>587</v>
-      </c>
-      <c r="F17" s="182" t="s">
-        <v>588</v>
-      </c>
       <c r="I17" s="63"/>
-      <c r="M17" s="63"/>
-      <c r="N17" s="63"/>
-      <c r="O17" s="63"/>
-      <c r="P17" s="63"/>
+      <c r="N17" s="68" t="s">
+        <v>438</v>
+      </c>
+      <c r="O17" s="68" t="s">
+        <v>359</v>
+      </c>
+      <c r="P17" s="68" t="s">
+        <v>360</v>
+      </c>
       <c r="Q17" s="63"/>
     </row>
     <row r="18" spans="1:17" s="68" customFormat="1">
@@ -17616,10 +17600,6 @@
       <c r="B18" s="182"/>
       <c r="C18" s="182"/>
       <c r="I18" s="63"/>
-      <c r="M18" s="63"/>
-      <c r="N18" s="63"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="63"/>
       <c r="Q18" s="63"/>
     </row>
     <row r="19" spans="1:17">
@@ -17627,10 +17607,16 @@
       <c r="J19" s="63"/>
       <c r="K19" s="63"/>
       <c r="L19" s="63"/>
-      <c r="M19" s="63"/>
-      <c r="N19" s="63"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="63"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68" t="s">
+        <v>467</v>
+      </c>
+      <c r="O19" s="68" t="s">
+        <v>468</v>
+      </c>
+      <c r="P19" s="68" t="s">
+        <v>469</v>
+      </c>
       <c r="Q19" s="63"/>
     </row>
     <row r="20" spans="1:17">
@@ -17638,10 +17624,10 @@
       <c r="J20" s="63"/>
       <c r="K20" s="63"/>
       <c r="L20" s="63"/>
-      <c r="M20" s="63"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="68"/>
+      <c r="P20" s="68"/>
       <c r="Q20" s="63"/>
     </row>
     <row r="21" spans="1:17">
@@ -17649,10 +17635,10 @@
       <c r="J21" s="63"/>
       <c r="K21" s="63"/>
       <c r="L21" s="63"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="63"/>
-      <c r="O21" s="63"/>
-      <c r="P21" s="63"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="68"/>
       <c r="Q21" s="63"/>
     </row>
     <row r="22" spans="1:17">
@@ -17660,10 +17646,10 @@
       <c r="J22" s="63"/>
       <c r="K22" s="63"/>
       <c r="L22" s="63"/>
-      <c r="M22" s="63"/>
-      <c r="N22" s="63"/>
-      <c r="O22" s="63"/>
-      <c r="P22" s="63"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="68"/>
+      <c r="P22" s="68"/>
       <c r="Q22" s="63"/>
     </row>
     <row r="23" spans="1:17">
@@ -17671,10 +17657,16 @@
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
       <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="63"/>
-      <c r="O23" s="63"/>
-      <c r="P23" s="63"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="182" t="s">
+        <v>636</v>
+      </c>
+      <c r="O23" s="68" t="s">
+        <v>525</v>
+      </c>
+      <c r="P23" s="68" t="s">
+        <v>526</v>
+      </c>
       <c r="Q23" s="63"/>
     </row>
     <row r="24" spans="1:17">
@@ -17682,10 +17674,10 @@
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
       <c r="L24" s="63"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="68"/>
       <c r="Q24" s="63"/>
     </row>
     <row r="25" spans="1:17">
@@ -17693,10 +17685,10 @@
       <c r="J25" s="63"/>
       <c r="K25" s="63"/>
       <c r="L25" s="63"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="63"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="63"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="68"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="68"/>
       <c r="Q25" s="63"/>
     </row>
     <row r="26" spans="1:17">
@@ -17704,10 +17696,16 @@
       <c r="J26" s="63"/>
       <c r="K26" s="63"/>
       <c r="L26" s="63"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="63"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="63"/>
+      <c r="M26" s="182"/>
+      <c r="N26" s="182" t="s">
+        <v>586</v>
+      </c>
+      <c r="O26" s="182" t="s">
+        <v>587</v>
+      </c>
+      <c r="P26" s="182" t="s">
+        <v>588</v>
+      </c>
       <c r="Q26" s="63"/>
     </row>
     <row r="27" spans="1:17">
@@ -17818,6 +17816,71 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="195" t="s">
+        <v>641</v>
+      </c>
+      <c r="B1" s="195" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="195" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="195" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="195" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="195" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="195" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="195" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="195" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="195" t="s">
+        <v>640</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -18008,10 +18071,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -18030,99 +18093,80 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
     </row>
+    <row r="2" spans="1:6" s="195" customFormat="1">
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+    </row>
     <row r="3" spans="1:6" ht="14.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="94" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="43"/>
-    </row>
-    <row r="4" spans="1:6" s="43" customFormat="1" ht="14.25">
-      <c r="A4" s="35" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="43"/>
+    </row>
+    <row r="5" spans="1:6" s="195" customFormat="1" ht="14.25">
+      <c r="A5" s="94" t="s">
+        <v>640</v>
+      </c>
+      <c r="B5" s="184"/>
+    </row>
+    <row r="6" spans="1:6" s="43" customFormat="1" ht="14.25">
+      <c r="A6" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B6" s="44" t="s">
         <v>345</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E6" s="43" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="12" t="s">
+    <row r="7" spans="1:6" ht="14.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="81" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>309</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>439</v>
-      </c>
-      <c r="D6" s="60" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="81" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A7" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>321</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>441</v>
-      </c>
-      <c r="D7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="53" customFormat="1" ht="14.25">
+    <row r="8" spans="1:6" s="81" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="B8" s="57" t="s">
-        <v>322</v>
-      </c>
-      <c r="C8" s="56" t="b">
-        <v>1</v>
+      <c r="B8" s="65" t="s">
+        <v>309</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>439</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>294</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="53" customFormat="1" ht="14.25" customHeight="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="81" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="57" t="s">
-        <v>323</v>
-      </c>
-      <c r="C9" s="56" t="s">
-        <v>308</v>
-      </c>
-      <c r="D9" s="60" t="s">
-        <v>295</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>319</v>
+      <c r="B9" s="65" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>441</v>
+      </c>
+      <c r="D9" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="53" customFormat="1" ht="14.25">
@@ -18130,196 +18174,212 @@
         <v>187</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="C10" s="56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="53" customFormat="1" ht="14.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="53" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="64" t="s">
         <v>187</v>
       </c>
       <c r="B11" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>295</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="53" customFormat="1" ht="14.25">
+      <c r="A12" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="C12" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>297</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="53" customFormat="1" ht="14.25">
+      <c r="A13" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="57" t="s">
         <v>324</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C13" s="56" t="s">
         <v>477</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D13" s="60" t="s">
         <v>298</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E13" s="53" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="81" customFormat="1" ht="14.25">
-      <c r="A12" s="64"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="60"/>
-    </row>
-    <row r="13" spans="1:6" s="81" customFormat="1" ht="14.25">
-      <c r="A13" s="64" t="s">
+    <row r="14" spans="1:6" s="81" customFormat="1" ht="14.25">
+      <c r="A14" s="64"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="60"/>
+    </row>
+    <row r="15" spans="1:6" s="81" customFormat="1" ht="14.25">
+      <c r="A15" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B15" s="81" t="s">
         <v>452</v>
       </c>
-      <c r="F13" s="121" t="s">
+      <c r="F15" s="121" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.25">
-      <c r="A14" s="35" t="s">
+    <row r="16" spans="1:6" ht="14.25">
+      <c r="A16" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B16" s="65" t="s">
         <v>453</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C16" s="56" t="s">
         <v>443</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D16" s="47" t="s">
         <v>329</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E16" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25">
-      <c r="A15" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="65" t="s">
-        <v>454</v>
-      </c>
-      <c r="C15" s="56" t="s">
-        <v>444</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>300</v>
-      </c>
-      <c r="E15" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.25">
-      <c r="A16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="65" t="s">
-        <v>455</v>
-      </c>
-      <c r="C16" s="37">
-        <v>13011111111</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>299</v>
-      </c>
-      <c r="E16" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="24">
+    <row r="17" spans="1:7" ht="14.25">
       <c r="A17" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>456</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>442</v>
+        <v>454</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>444</v>
       </c>
       <c r="D17" s="47" t="s">
-        <v>251</v>
+        <v>300</v>
       </c>
       <c r="E17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25">
       <c r="A18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>455</v>
+      </c>
+      <c r="C18" s="37">
+        <v>13011111111</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="E18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="24">
+      <c r="A19" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>456</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>442</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="E19" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.25">
+      <c r="A20" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B20" s="65" t="s">
         <v>457</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C20" s="56" t="s">
         <v>445</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D20" s="47" t="s">
         <v>311</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="81" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A19" s="125" t="s">
+    <row r="21" spans="1:7" s="81" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A21" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="159" t="s">
+      <c r="B21" s="159" t="s">
         <v>530</v>
       </c>
-      <c r="C19" s="159"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159" t="s">
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159" t="s">
         <v>531</v>
       </c>
-      <c r="G19" s="159"/>
-    </row>
-    <row r="20" spans="1:7" s="81" customFormat="1"/>
-    <row r="21" spans="1:7" ht="14.25">
-      <c r="A21" s="15" t="s">
+      <c r="G21" s="159"/>
+    </row>
+    <row r="22" spans="1:7" s="81" customFormat="1"/>
+    <row r="23" spans="1:7" ht="14.25">
+      <c r="A23" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>252</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E23" s="16" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.25">
-      <c r="A22" s="64" t="s">
+    <row r="24" spans="1:7" ht="14.25">
+      <c r="A24" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="B22" s="183" t="s">
+      <c r="B24" s="183" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="B24" s="53"/>
-    </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="81"/>
-      <c r="C26" s="81"/>
+      <c r="B26" s="53"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="A28" s="81"/>
+      <c r="C28" s="81"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="13"/>
@@ -18344,15 +18404,33 @@
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C17" r:id="rId1"/>
+    <hyperlink ref="C19" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -22542,10 +22620,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -22563,12 +22641,10 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3" s="176" t="s">
-        <v>258</v>
-      </c>
-      <c r="B3" s="195" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25">
@@ -22576,66 +22652,79 @@
         <v>258</v>
       </c>
       <c r="B4" s="195" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25">
+      <c r="A5" s="176" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.25">
+      <c r="A6" s="176" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" s="195" t="s">
         <v>345</v>
       </c>
-      <c r="G4" s="195" t="s">
+      <c r="G6" s="195" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25">
-      <c r="A5" s="176"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
-      <c r="A6" s="176" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="179" t="s">
-        <v>637</v>
-      </c>
-      <c r="C6" s="178" t="s">
-        <v>524</v>
-      </c>
-      <c r="D6" s="180" t="s">
-        <v>521</v>
-      </c>
-      <c r="F6" s="122"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
-      <c r="A7" s="176" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="179" t="s">
-        <v>520</v>
-      </c>
-      <c r="C7" s="178" t="s">
-        <v>523</v>
-      </c>
-      <c r="D7" s="180" t="s">
-        <v>301</v>
-      </c>
-      <c r="F7" s="122"/>
+    <row r="7" spans="1:7" ht="14.25">
+      <c r="A7" s="176"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" s="176" t="s">
-        <v>258</v>
+        <v>187</v>
       </c>
       <c r="B8" s="179" t="s">
-        <v>532</v>
-      </c>
-      <c r="C8" s="178"/>
-      <c r="D8" s="180"/>
-      <c r="F8" s="122" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.25">
+        <v>637</v>
+      </c>
+      <c r="C8" s="178" t="s">
+        <v>524</v>
+      </c>
+      <c r="D8" s="180" t="s">
+        <v>521</v>
+      </c>
+      <c r="F8" s="122"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1">
+      <c r="A9" s="176" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="179" t="s">
+        <v>520</v>
+      </c>
+      <c r="C9" s="178" t="s">
+        <v>523</v>
+      </c>
+      <c r="D9" s="180" t="s">
+        <v>301</v>
+      </c>
+      <c r="F9" s="122"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="176" t="s">
         <v>258</v>
       </c>
-      <c r="B10" s="195" t="s">
+      <c r="B10" s="179" t="s">
+        <v>532</v>
+      </c>
+      <c r="C10" s="178"/>
+      <c r="D10" s="180"/>
+      <c r="F10" s="122" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.25">
+      <c r="A12" s="176" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="195" t="s">
         <v>252</v>
       </c>
-      <c r="E10" s="195" t="s">
+      <c r="E12" s="195" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>